<commit_message>
added db table design details in new sheet
</commit_message>
<xml_diff>
--- a/db_table_design.xlsx
+++ b/db_table_design.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\construction\myprojects\treesurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544ED41A-5469-423F-8FF4-C2A1126BA3B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6FB6CC-542C-479D-8E6A-3049DFD6EC8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="rev_2" sheetId="2" r:id="rId2"/>
+    <sheet name="postgres_db_design" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
   <si>
     <t>Experiment</t>
   </si>
@@ -94,13 +96,157 @@
   </si>
   <si>
     <t>10CGD</t>
+  </si>
+  <si>
+    <t>experiment</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>surveyor_master</t>
+  </si>
+  <si>
+    <t>treeId</t>
+  </si>
+  <si>
+    <t>inspection_date</t>
+  </si>
+  <si>
+    <t>Health_score</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>planting_date</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>Treeid</t>
+  </si>
+  <si>
+    <t>Tree_master</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Nilgiri</t>
+  </si>
+  <si>
+    <t>Not healthy</t>
+  </si>
+  <si>
+    <t>exp1</t>
+  </si>
+  <si>
+    <t>site1</t>
+  </si>
+  <si>
+    <t>locationId</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>site2</t>
+  </si>
+  <si>
+    <t>exp2</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>date picker</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>data driven</t>
+  </si>
+  <si>
+    <t>from UI</t>
+  </si>
+  <si>
+    <t>datepicker</t>
+  </si>
+  <si>
+    <t>pathogen_count</t>
+  </si>
+  <si>
+    <t>wood_borer_cound</t>
+  </si>
+  <si>
+    <t>ignore</t>
+  </si>
+  <si>
+    <t>string-20</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string - 500</t>
+  </si>
+  <si>
+    <t>string - 20</t>
+  </si>
+  <si>
+    <t>String - 100</t>
+  </si>
+  <si>
+    <t>string - 100</t>
+  </si>
+  <si>
+    <t>String 200</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +269,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,8 +297,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -182,11 +348,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -202,6 +383,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,4 +827,680 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A831AF99-3C86-4F50-B9E1-08E550B86488}">
+  <dimension ref="A1:R20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="8.88671875" style="6"/>
+    <col min="14" max="14" width="14.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="G1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="M1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="9">
+        <v>44470</v>
+      </c>
+      <c r="O3" s="7">
+        <v>2</v>
+      </c>
+      <c r="P3" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>12</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="7"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="9">
+        <v>44197</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="F20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE29C97-BD39-44F2-B4A0-2FFDDB89C09F}">
+  <dimension ref="A1:R15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="8.88671875" style="6"/>
+    <col min="14" max="14" width="14.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="G1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="M1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="9">
+        <v>44470</v>
+      </c>
+      <c r="O3" s="7">
+        <v>2</v>
+      </c>
+      <c r="P3" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>12</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="M4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="M5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="9">
+        <v>44197</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="E10:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>